<commit_message>
more links fixed. Emissions and labour links added. EMOD running
</commit_message>
<xml_diff>
--- a/EmissionFactors.xlsx
+++ b/EmissionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\KENTIMGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C15F9-F5D2-4CF5-BCC2-F3CA3C94A3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA9332F-BFCF-4657-90AB-5A02139ADF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27720" windowHeight="14715" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="1382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="1390">
   <si>
     <t>Source GHG: IPPC National GHG Guideline 2006 - kTon/PJ = ton/TJ</t>
   </si>
@@ -4288,16 +4288,40 @@
     <t>PWROKE</t>
   </si>
   <si>
-    <t>GHCO00</t>
-  </si>
-  <si>
-    <t>GHDS00</t>
-  </si>
-  <si>
-    <t>GHHF00</t>
-  </si>
-  <si>
-    <t>GHNG00</t>
+    <t>KECO00</t>
+  </si>
+  <si>
+    <t>KEDS00</t>
+  </si>
+  <si>
+    <t>KEHF00</t>
+  </si>
+  <si>
+    <t>KENG00</t>
+  </si>
+  <si>
+    <t>KENG01</t>
+  </si>
+  <si>
+    <t>KENG02</t>
+  </si>
+  <si>
+    <t>KENG04</t>
+  </si>
+  <si>
+    <t>KEDS02</t>
+  </si>
+  <si>
+    <t>KEDS03</t>
+  </si>
+  <si>
+    <t>KEDS04</t>
+  </si>
+  <si>
+    <t>KEDS06</t>
+  </si>
+  <si>
+    <t>KEDS09</t>
   </si>
 </sst>
 </file>
@@ -4307,7 +4331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4374,6 +4398,12 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4957,7 +4987,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B5,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B5,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Biogas                               </v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4994,7 +5024,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B6,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B6,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Bioethanol                          </v>
       </c>
       <c r="B6" s="1" t="s">
@@ -5031,7 +5061,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B7,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B7,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Biodiesel                           </v>
       </c>
       <c r="B7" s="1" t="s">
@@ -5068,7 +5098,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B8,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B8,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Industry - Biomass Bagasse                        </v>
       </c>
       <c r="B8" s="1" t="s">
@@ -5105,7 +5135,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B9,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B9,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Biomass Other                        </v>
       </c>
       <c r="B9" s="1" t="s">
@@ -5142,7 +5172,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B10,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B10,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Industry - Biomass wood                           </v>
       </c>
       <c r="B10" s="1" t="s">
@@ -5179,7 +5209,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B11,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B11,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Coal                                  </v>
       </c>
       <c r="B11" s="1" t="s">
@@ -5216,7 +5246,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B12,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B12,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Industry - Coking coal                            </v>
       </c>
       <c r="B12" s="1" t="s">
@@ -5253,7 +5283,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B13,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B13,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Industry - Iron and Steel - Coking coal           </v>
       </c>
       <c r="B13" t="s">
@@ -5298,7 +5328,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B14,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B14,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Coal Discard                         </v>
       </c>
       <c r="B14" s="1" t="s">
@@ -5335,7 +5365,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B15,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B15,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Coal low grade                       </v>
       </c>
       <c r="B15" s="1" t="s">
@@ -5372,7 +5402,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B16,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B16,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Coal low grade - waterberg           </v>
       </c>
       <c r="B16" t="s">
@@ -5409,7 +5439,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B17,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B17,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B17" t="s">
@@ -5446,7 +5476,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B18,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B18,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B18" t="s">
@@ -5483,7 +5513,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B19,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B19,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B19" t="s">
@@ -5520,7 +5550,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B20,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B20,ForGams!$J$3:$J$602,0))</f>
         <v>Matla Coal</v>
       </c>
       <c r="B20" t="s">
@@ -5557,7 +5587,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B21,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B21,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B21" t="s">
@@ -5594,7 +5624,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B22,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B22,ForGams!$J$3:$J$602,0))</f>
         <v>Kriel Coal</v>
       </c>
       <c r="B22" t="s">
@@ -5631,7 +5661,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B23,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B23,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Heat-Steam New                      </v>
       </c>
       <c r="B23" t="s">
@@ -5668,7 +5698,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B24,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B24,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B24" t="s">
@@ -5705,7 +5735,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B25,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B25,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve"> Arnot Coal</v>
       </c>
       <c r="B25" t="s">
@@ -5742,7 +5772,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B26,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B26,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B26" t="s">
@@ -5779,7 +5809,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B27,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B27,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B27" t="s">
@@ -5816,7 +5846,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B28,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B28,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B28" t="s">
@@ -5853,7 +5883,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B29,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B29,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve"> Grootegeluk Coal</v>
       </c>
       <c r="B29" t="s">
@@ -5890,7 +5920,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B30,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B30,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B30" t="s">
@@ -5927,7 +5957,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B31,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B31,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B31" t="s">
@@ -5964,7 +5994,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B32,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B32,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Coal for plants in Botswana          </v>
       </c>
       <c r="B32" s="5" t="s">
@@ -6001,7 +6031,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B33,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B33,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Electricity                           </v>
       </c>
       <c r="B33" s="1" t="s">
@@ -6038,7 +6068,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B34,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B34,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -6075,7 +6105,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B35,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B35,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Commercial - Gas                                  </v>
       </c>
       <c r="B35" s="1" t="s">
@@ -6112,7 +6142,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B36,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B36,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Gas Southern Mozambique              </v>
       </c>
       <c r="B36" s="5" t="s">
@@ -6149,7 +6179,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B37,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B37,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Gas Namibia                          </v>
       </c>
       <c r="B37" s="5" t="s">
@@ -6186,7 +6216,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B38,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B38,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -6223,7 +6253,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B39,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B39,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -6260,7 +6290,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B40,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B40,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Gas Northern Mozambique              </v>
       </c>
       <c r="B40" s="5" t="s">
@@ -6297,7 +6327,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B41,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B41,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -6334,7 +6364,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B42,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B42,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Gas Indigenous Shale                 </v>
       </c>
       <c r="B42" s="1" t="s">
@@ -6371,7 +6401,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B43,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B43,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Coastal Gas                          </v>
       </c>
       <c r="B43" s="1" t="s">
@@ -6408,7 +6438,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B44,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B44,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -6445,7 +6475,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B45,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B45,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -6482,7 +6512,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B46,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B46,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Heat-Steam Existing                 </v>
       </c>
       <c r="B46" s="1" t="s">
@@ -6519,7 +6549,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B47,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B47,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Heat-Steam New                      </v>
       </c>
       <c r="B47" s="1" t="s">
@@ -6556,7 +6586,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B48,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B48,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Hydro                                </v>
       </c>
       <c r="B48" s="1" t="s">
@@ -6593,7 +6623,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B49,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B49,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Transport Hydrogen                                </v>
       </c>
       <c r="B49" s="6" t="s">
@@ -6630,7 +6660,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B50,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B50,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Nuclear                              </v>
       </c>
       <c r="B50" s="1" t="s">
@@ -6667,7 +6697,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B51,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B51,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Transport Oil Av Gasoline                         </v>
       </c>
       <c r="B51" s="1" t="s">
@@ -6704,7 +6734,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B52,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B52,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Supply Sector Oil Crude                           </v>
       </c>
       <c r="B52" s="1" t="s">
@@ -6741,7 +6771,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B53,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B53,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Oil Diesel                            </v>
       </c>
       <c r="B53" s="1" t="s">
@@ -6778,7 +6808,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B54,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B54,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Oil Gasoline                          </v>
       </c>
       <c r="B54" s="1" t="s">
@@ -6815,7 +6845,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B55,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B55,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Oil HFO                               </v>
       </c>
       <c r="B55" s="1" t="s">
@@ -6852,7 +6882,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B56,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B56,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Oil Kerosene                          </v>
       </c>
       <c r="B56" s="1" t="s">
@@ -6889,7 +6919,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B57,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B57,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Agriculture Oil LPG                               </v>
       </c>
       <c r="B57" s="1" t="s">
@@ -6926,7 +6956,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="e">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B58,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B58,ForGams!$J$3:$J$602,0))</f>
         <v>#N/A</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -6963,7 +6993,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B59,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B59,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Solar                                </v>
       </c>
       <c r="B59" s="1" t="s">
@@ -7000,7 +7030,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B60,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B60,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Power Sector Wind                                 </v>
       </c>
       <c r="B60" s="1" t="s">
@@ -7037,7 +7067,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>INDEX(ForGams!$L$3:$L$603,MATCH(B61,ForGams!$J$3:$J$603,0))</f>
+        <f>INDEX(ForGams!$L$3:$L$602,MATCH(B61,ForGams!$J$3:$J$602,0))</f>
         <v xml:space="preserve">Industry - Waste                                  </v>
       </c>
       <c r="B61" s="1" t="s">
@@ -7081,10 +7111,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA525E55-6D10-45A0-86EF-16765CC6C762}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="C1:AF484"/>
+  <dimension ref="C1:AF492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
-      <selection activeCell="D483" sqref="D483:G483"/>
+      <selection activeCell="D481" sqref="D481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31368,11 +31398,148 @@
         <v>56.152000000000001</v>
       </c>
     </row>
+    <row r="485" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C485" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D485">
+        <v>56.1</v>
+      </c>
+      <c r="E485">
+        <v>1E-3</v>
+      </c>
+      <c r="F485">
+        <v>1E-4</v>
+      </c>
+      <c r="G485">
+        <v>56.152000000000001</v>
+      </c>
+    </row>
+    <row r="486" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C486" t="s">
+        <v>1383</v>
+      </c>
+      <c r="D486">
+        <v>56.1</v>
+      </c>
+      <c r="E486">
+        <v>1E-3</v>
+      </c>
+      <c r="F486">
+        <v>1E-4</v>
+      </c>
+      <c r="G486">
+        <v>56.152000000000001</v>
+      </c>
+    </row>
+    <row r="487" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C487" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D487">
+        <v>56.1</v>
+      </c>
+      <c r="E487">
+        <v>1E-3</v>
+      </c>
+      <c r="F487">
+        <v>1E-4</v>
+      </c>
+      <c r="G487">
+        <v>56.152000000000001</v>
+      </c>
+    </row>
+    <row r="488" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C488" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D488">
+        <v>74.066699999999997</v>
+      </c>
+      <c r="E488">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F488">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G488">
+        <v>74.315700000000007</v>
+      </c>
+    </row>
+    <row r="489" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C489" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D489">
+        <v>74.066699999999997</v>
+      </c>
+      <c r="E489">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F489">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G489">
+        <v>74.315700000000007</v>
+      </c>
+    </row>
+    <row r="490" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C490" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D490">
+        <v>74.066699999999997</v>
+      </c>
+      <c r="E490">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F490">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G490">
+        <v>74.315700000000007</v>
+      </c>
+    </row>
+    <row r="491" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C491" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D491">
+        <v>74.066699999999997</v>
+      </c>
+      <c r="E491">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F491">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G491">
+        <v>74.315700000000007</v>
+      </c>
+    </row>
+    <row r="492" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C492" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D492">
+        <v>74.066699999999997</v>
+      </c>
+      <c r="E492">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F492">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G492">
+        <v>74.315700000000007</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="C1:G480" xr:uid="{661748B0-3AD1-481C-B04F-26CCFCAA4FD8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AC3:AD55">
     <sortCondition ref="AC3:AC55"/>
   </sortState>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>